<commit_message>
clueSetup updated with player information
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdiam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charliedupras/eclipse-workspace/Clue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62553E5-AECD-49AE-88A4-9780FA3878AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F27712-9132-E845-82C5-9986842F7ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{551E4A14-F6D3-400B-B156-65F435F96048}"/>
+    <workbookView xWindow="11940" yWindow="500" windowWidth="23900" windowHeight="10960" xr2:uid="{551E4A14-F6D3-400B-B156-65F435F96048}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +168,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +228,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -213,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,6 +262,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -248,9 +300,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -288,7 +340,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -394,7 +446,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -536,7 +588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -546,16 +598,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7C5659-757F-4CD1-9D86-CBC1835105D8}">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="113" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="31" width="5.6796875" customWidth="1"/>
+    <col min="1" max="31" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>1</v>
@@ -648,7 +700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -743,7 +795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -777,7 +829,7 @@
       <c r="K3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -838,7 +890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -933,7 +985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1028,7 +1080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1123,7 +1175,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1218,7 +1270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1313,7 +1365,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1408,7 +1460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1503,7 +1555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1598,14 +1650,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1686,14 +1738,14 @@
       <c r="AC12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AD12" s="4" t="s">
+      <c r="AD12" s="7" t="s">
         <v>0</v>
       </c>
       <c r="AE12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1788,7 +1840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1883,7 +1935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1978,7 +2030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2073,7 +2125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2168,7 +2220,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2263,7 +2315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2358,7 +2410,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2389,7 +2441,7 @@
       <c r="J20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="11" t="s">
         <v>0</v>
       </c>
       <c r="L20" s="4" t="s">
@@ -2453,7 +2505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2548,7 +2600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2643,7 +2695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2738,7 +2790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2833,7 +2885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2928,7 +2980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3023,7 +3075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3118,7 +3170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3213,7 +3265,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3308,7 +3360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3336,7 +3388,7 @@
       <c r="I30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="10" t="s">
         <v>0</v>
       </c>
       <c r="K30" s="3" t="s">
@@ -3396,14 +3448,14 @@
       <c r="AC30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AD30" s="4" t="s">
+      <c r="AD30" s="6" t="s">
         <v>0</v>
       </c>
       <c r="AE30" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>

</xml_diff>